<commit_message>
Updated Entry cost, cost, mass & amount of storage for the 5 round tanks  Update spreadsheet in docs with round tank values on new page
</commit_message>
<xml_diff>
--- a/Documentation/PartsBalance.xlsx
+++ b/Documentation/PartsBalance.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jbb\github\IFI-Life-Support\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC43F10-523B-412A-9FBE-B740210F6B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39BF2E0-2FF6-4234-81CA-AFFDB935BF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19305" yWindow="3450" windowWidth="18255" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23040" yWindow="780" windowWidth="15360" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Round Tanks" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t>PartName</t>
   </si>
@@ -178,6 +190,42 @@
   </si>
   <si>
     <t>Locked K&amp;B tanks are automatically used for vessels on rails</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>(multiplier)</t>
+  </si>
+  <si>
+    <t>Entry cost</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Total Surface Area</t>
+  </si>
+  <si>
+    <t>K&amp;B</t>
+  </si>
+  <si>
+    <t>K&amp;B/unit volume</t>
   </si>
 </sst>
 </file>
@@ -227,10 +275,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -528,7 +576,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -573,7 +621,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -625,7 +673,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -639,20 +687,20 @@
       <c r="C24" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
@@ -903,4 +951,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC534F1F-E6D2-42D9-9860-501E792DC580}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1">
+        <v>1.25</v>
+      </c>
+      <c r="E1">
+        <v>1.875</v>
+      </c>
+      <c r="F1">
+        <v>2.5</v>
+      </c>
+      <c r="G1">
+        <v>3.75</v>
+      </c>
+      <c r="H1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <f>D1/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:H2" si="0">E1/2</f>
+        <v>0.9375</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>1.875</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <f>D1/3</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E3">
+        <f>E11*$D$3</f>
+        <v>0.625</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:H3" si="1">F11*$D$3</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <f>PI()*D2^2</f>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="E4">
+        <f>PI()*E2^2</f>
+        <v>2.7611654181941541</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:H4" si="2">PI()*F2^2</f>
+        <v>4.908738521234052</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>11.044661672776616</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>19.634954084936208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5">
+        <f>PI()*D2^2*D3</f>
+        <v>0.51132692929521373</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:H5" si="3">PI()*E2^2*E3</f>
+        <v>1.7257283863713462</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>4.0906154343617098</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>13.805827090970769</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>32.724923474893679</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6">
+        <f>2*PI()*(D1/2)*D3+2*PI()*D2^2</f>
+        <v>4.0906154343617098</v>
+      </c>
+      <c r="E6">
+        <f>2*PI()*(E1/2)*E3+2*PI()*E2^2</f>
+        <v>9.2038847273138469</v>
+      </c>
+      <c r="F6">
+        <f>2*PI()*(F1/2)*F3+2*PI()*F2^2</f>
+        <v>16.362461737446839</v>
+      </c>
+      <c r="G6">
+        <f>2*PI()*(G1/2)*G3+2*PI()*G2^2</f>
+        <v>36.815538909255388</v>
+      </c>
+      <c r="H6">
+        <f>2*PI()*(H1/2)*H3+2*PI()*H2^2</f>
+        <v>65.449846949787357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <f>D16/D5</f>
+        <v>97.784797035660503</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11">
+        <f>E1/$D$1</f>
+        <v>1.5</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:H11" si="4">F1/$D$1</f>
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13">
+        <v>2500</v>
+      </c>
+      <c r="E13">
+        <f>E11^2*$D$14</f>
+        <v>2700</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:H13" si="5">F11^2*$D$14</f>
+        <v>4800</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>10800</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="5"/>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>1200</v>
+      </c>
+      <c r="E14">
+        <f>$E$11*D14</f>
+        <v>1800</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:H14" si="6">$E$11*E14</f>
+        <v>2700</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="6"/>
+        <v>4050</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15">
+        <v>0.06</v>
+      </c>
+      <c r="E15">
+        <f>$D$15/$D$6*E6</f>
+        <v>0.13499999999999998</v>
+      </c>
+      <c r="F15">
+        <f>$D$15/$D$6*F6</f>
+        <v>0.24</v>
+      </c>
+      <c r="G15">
+        <f>$D$15/$D$6*G6</f>
+        <v>0.53999999999999992</v>
+      </c>
+      <c r="H15">
+        <f>$D$15/$D$6*H6</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <f>E5*$D$7</f>
+        <v>168.75</v>
+      </c>
+      <c r="F16">
+        <f>F5*$D$7</f>
+        <v>400</v>
+      </c>
+      <c r="G16">
+        <f>G5*$D$7</f>
+        <v>1350</v>
+      </c>
+      <c r="H16">
+        <f>H5*$D$7</f>
+        <v>3200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>